<commit_message>
changed alexis plane aoa graph
</commit_message>
<xml_diff>
--- a/aoa_graphs/aoa_graphs.xlsx
+++ b/aoa_graphs/aoa_graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1whoh\Files2\Code\eclipse-projects\discord_bots\DiamondStarCombat-1.18.2\aoa_graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1whoh\Files2\Code\eclipse-projects\discord_bots\DiamondStarCombat\aoa_graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CFAEA8-4C87-4E55-8E3F-2EE09013B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885130D7-DAC5-4C3E-8E0C-941631D2F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Alexis Plane</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>Lift Coefficient</t>
+  </si>
+  <si>
+    <t>Javi Plane</t>
+  </si>
+  <si>
+    <t>Wooden Plane</t>
+  </si>
+  <si>
+    <t>E3Sentry Plane</t>
   </si>
 </sst>
 </file>
@@ -201,179 +210,251 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$29</c:f>
+              <c:f>Sheet1!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>-18</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-17</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="12">
                   <c:v>-16</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>-14</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>-12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="16">
                   <c:v>-8</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>-6</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>-4</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>-2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="25">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="26">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="29">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="30">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$29</c:f>
+              <c:f>Sheet1!$B$3:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
+                <c:ptCount val="41"/>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-0.78</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>-1.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
+                  <c:v>-1.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>-1.1499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1.18</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>-1.1100000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
+                  <c:v>-1.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>-0.99</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.84</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.69</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
+                  <c:v>-0.89</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.79</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>-0.48</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.25</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
+                  <c:v>-0.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.69</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.99</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="29">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>1.1100000000000001</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="31">
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="32">
                   <c:v>1.18</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="33">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>1.04</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="36">
                   <c:v>0.78</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="37">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -573,7 +654,1540 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Javi Plane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lift Coefficient</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C27-4C47-915C-70C4FF48B849}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1753924639"/>
+        <c:axId val="1510139999"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1753924639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510139999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1510139999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1753924639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$61:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Wooden Plane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lift Coefficient</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$63:$A$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$63:$B$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A84-4851-97A7-A6591FA79D5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1577258815"/>
+        <c:axId val="1567204319"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1577258815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1567204319"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1567204319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1577258815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$61:$L$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>E3Sentry Plane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lift Coefficient</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$63:$K$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$63:$L$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCB3-489D-A74B-6F7ABE1396DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1752243967"/>
+        <c:axId val="1569591727"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1752243967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1569591727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1569591727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1752243967"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1129,20 +2743,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1162,6 +4324,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2C1C7B1-636C-89F0-6935-46CE8F971D55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84940A52-42AC-CE01-ED6D-06B293FF6E79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A52503-6855-AB73-2187-B55935BA312F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1433,10 +4703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,233 +4715,936 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>-40</v>
+      </c>
+      <c r="K3">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-38</v>
+      </c>
+      <c r="K4">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-36</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>-26</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-34</v>
+      </c>
+      <c r="B6">
+        <v>-0.4</v>
+      </c>
+      <c r="K6">
+        <v>-24</v>
+      </c>
+      <c r="L6">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-32</v>
+      </c>
+      <c r="B7">
+        <v>-0.78</v>
+      </c>
+      <c r="K7">
+        <v>-22</v>
+      </c>
+      <c r="L7">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-30</v>
+      </c>
+      <c r="B8">
+        <v>-1.04</v>
+      </c>
+      <c r="K8">
         <v>-20</v>
       </c>
-      <c r="B3">
+      <c r="L8">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-28</v>
+      </c>
+      <c r="B9">
+        <v>-1.18</v>
+      </c>
+      <c r="K9">
+        <v>-18</v>
+      </c>
+      <c r="L9">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-26</v>
+      </c>
+      <c r="B10">
+        <v>-1.2</v>
+      </c>
+      <c r="K10">
+        <v>-16</v>
+      </c>
+      <c r="L10">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-24</v>
+      </c>
+      <c r="B11">
+        <v>-1.18</v>
+      </c>
+      <c r="K11">
+        <v>-14</v>
+      </c>
+      <c r="L11">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-22</v>
+      </c>
+      <c r="B12">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="K12">
+        <v>-12</v>
+      </c>
+      <c r="L12">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-20</v>
+      </c>
+      <c r="B13">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="K13">
+        <v>-10</v>
+      </c>
+      <c r="L13">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-18</v>
+      </c>
+      <c r="B14">
+        <v>-1.06</v>
+      </c>
+      <c r="K14">
+        <v>-8</v>
+      </c>
+      <c r="L14">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-16</v>
+      </c>
+      <c r="B15">
+        <v>-0.99</v>
+      </c>
+      <c r="K15">
+        <v>-6</v>
+      </c>
+      <c r="L15">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-14</v>
+      </c>
+      <c r="B16">
+        <v>-0.89</v>
+      </c>
+      <c r="K16">
+        <v>-4</v>
+      </c>
+      <c r="L16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-12</v>
+      </c>
+      <c r="B17">
+        <v>-0.79</v>
+      </c>
+      <c r="K17">
+        <v>-2</v>
+      </c>
+      <c r="L17">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-10</v>
+      </c>
+      <c r="B18">
+        <v>-0.68</v>
+      </c>
+      <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="L18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-8</v>
+      </c>
+      <c r="B19">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-6</v>
+      </c>
+      <c r="B20">
+        <v>-0.48</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-4</v>
+      </c>
+      <c r="B21">
+        <v>-0.36</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-2</v>
+      </c>
+      <c r="B22">
+        <v>-0.2</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+      <c r="L22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>0.2</v>
+      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+      <c r="L24">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>0.36</v>
+      </c>
+      <c r="K25">
+        <v>14</v>
+      </c>
+      <c r="L25">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>0.48</v>
+      </c>
+      <c r="K26">
+        <v>16</v>
+      </c>
+      <c r="L26">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K27">
+        <v>18</v>
+      </c>
+      <c r="L27">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>0.68</v>
+      </c>
+      <c r="K28">
+        <v>20</v>
+      </c>
+      <c r="L28">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>0.79</v>
+      </c>
+      <c r="K29">
+        <v>22</v>
+      </c>
+      <c r="L29">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>0.89</v>
+      </c>
+      <c r="K30">
+        <v>24</v>
+      </c>
+      <c r="L30">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>0.99</v>
+      </c>
+      <c r="K31">
+        <v>26</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>1.06</v>
+      </c>
+      <c r="K32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>22</v>
+      </c>
+      <c r="B34">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>26</v>
+      </c>
+      <c r="B36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="K61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="K62" t="s">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-20</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>-18</v>
       </c>
-      <c r="B4">
+      <c r="B64">
         <v>-0.78</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="K64">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>-17</v>
       </c>
-      <c r="B5">
+      <c r="B65">
         <v>-1.04</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="K65">
+        <v>-26</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>-16</v>
       </c>
-      <c r="B6">
+      <c r="B66">
         <v>-1.1499999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="K66">
+        <v>-24</v>
+      </c>
+      <c r="L66">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>-15</v>
       </c>
-      <c r="B7">
+      <c r="B67">
         <v>-1.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="K67">
+        <v>-22</v>
+      </c>
+      <c r="L67">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>-14</v>
       </c>
-      <c r="B8">
+      <c r="B68">
         <v>-1.18</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="K68">
+        <v>-20</v>
+      </c>
+      <c r="L68">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>-13</v>
       </c>
-      <c r="B9">
+      <c r="B69">
         <v>-1.1499999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="K69">
+        <v>-18</v>
+      </c>
+      <c r="L69">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>-12</v>
       </c>
-      <c r="B10">
+      <c r="B70">
         <v>-1.1100000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="K70">
+        <v>-16</v>
+      </c>
+      <c r="L70">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>-10</v>
       </c>
-      <c r="B11">
+      <c r="B71">
         <v>-0.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="K71">
+        <v>-14</v>
+      </c>
+      <c r="L71">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>-8</v>
       </c>
-      <c r="B12">
+      <c r="B72">
         <v>-0.84</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="K72">
+        <v>-12</v>
+      </c>
+      <c r="L72">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>-6</v>
       </c>
-      <c r="B13">
+      <c r="B73">
         <v>-0.69</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="K73">
+        <v>-10</v>
+      </c>
+      <c r="L73">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>-4</v>
       </c>
-      <c r="B14">
+      <c r="B74">
         <v>-0.48</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="K74">
+        <v>-8</v>
+      </c>
+      <c r="L74">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>-2</v>
       </c>
-      <c r="B15">
+      <c r="B75">
         <v>-0.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="K75">
+        <v>-6</v>
+      </c>
+      <c r="L75">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="B76">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="K76">
+        <v>-4</v>
+      </c>
+      <c r="L76">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>2</v>
       </c>
-      <c r="B17">
+      <c r="B77">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="K77">
+        <v>-2</v>
+      </c>
+      <c r="L77">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B78">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>6</v>
       </c>
-      <c r="B19">
+      <c r="B79">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="K79">
+        <v>2</v>
+      </c>
+      <c r="L79">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>8</v>
       </c>
-      <c r="B20">
+      <c r="B80">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="K80">
+        <v>4</v>
+      </c>
+      <c r="L80">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>10</v>
       </c>
-      <c r="B21">
+      <c r="B81">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="K81">
+        <v>6</v>
+      </c>
+      <c r="L81">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>12</v>
       </c>
-      <c r="B22">
+      <c r="B82">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="K82">
+        <v>8</v>
+      </c>
+      <c r="L82">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>13</v>
       </c>
-      <c r="B23">
+      <c r="B83">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="K83">
+        <v>10</v>
+      </c>
+      <c r="L83">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>14</v>
       </c>
-      <c r="B24">
+      <c r="B84">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="K84">
+        <v>12</v>
+      </c>
+      <c r="L84">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>15</v>
       </c>
-      <c r="B25">
+      <c r="B85">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="K85">
+        <v>14</v>
+      </c>
+      <c r="L85">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>16</v>
       </c>
-      <c r="B26">
+      <c r="B86">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="K86">
+        <v>16</v>
+      </c>
+      <c r="L86">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>17</v>
       </c>
-      <c r="B27">
+      <c r="B87">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="K87">
         <v>18</v>
       </c>
-      <c r="B28">
+      <c r="L87">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>18</v>
+      </c>
+      <c r="B88">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="K88">
         <v>20</v>
       </c>
-      <c r="B29">
+      <c r="L88">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>20</v>
+      </c>
+      <c r="B89">
         <v>0</v>
+      </c>
+      <c r="K89">
+        <v>22</v>
+      </c>
+      <c r="L89">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <v>24</v>
+      </c>
+      <c r="L90">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K91">
+        <v>26</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K92">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K93">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed javi and e3sentry aoa lift graph
</commit_message>
<xml_diff>
--- a/aoa_graphs/aoa_graphs.xlsx
+++ b/aoa_graphs/aoa_graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1whoh\Files2\Code\eclipse-projects\discord_bots\DiamondStarCombat\aoa_graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885130D7-DAC5-4C3E-8E0C-941631D2F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7848B168-37DB-47A2-812D-33FA17942440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1865,7 +1865,7 @@
                   <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -4705,8 +4705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="G61" zoomScale="72" workbookViewId="0">
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,7 +5626,7 @@
         <v>24</v>
       </c>
       <c r="L90">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
jason and wooden plane have more stable aoa
</commit_message>
<xml_diff>
--- a/aoa_graphs/aoa_graphs.xlsx
+++ b/aoa_graphs/aoa_graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1whoh\Files2\Code\eclipse-projects\discord_bots\DiamondStarCombat\aoa_graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1whoh\Files\Creative\Minecrap\Mod_Develope\DiamondStarCombat\aoa_graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7848B168-37DB-47A2-812D-33FA17942440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58775F2F-0EE5-4286-90F2-F98950644DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5655" yWindow="1425" windowWidth="17190" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1318,79 +1318,79 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.78</c:v>
+                  <c:v>-0.72</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>-0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>-1.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.2</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.18</c:v>
+                  <c:v>-1.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.1499999999999999</c:v>
+                  <c:v>-0.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.1100000000000001</c:v>
+                  <c:v>-0.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.99</c:v>
+                  <c:v>-0.82</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.84</c:v>
+                  <c:v>-0.68</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.69</c:v>
+                  <c:v>-0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.48</c:v>
+                  <c:v>-0.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.25</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.48</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.69</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.84</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.18</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.04</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.78</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -4705,8 +4705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G61" zoomScale="72" workbookViewId="0">
-      <selection activeCell="L91" sqref="L91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="72" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5265,7 +5265,7 @@
         <v>-18</v>
       </c>
       <c r="B64">
-        <v>-0.78</v>
+        <v>-0.72</v>
       </c>
       <c r="K64">
         <v>-28</v>
@@ -5276,7 +5276,7 @@
         <v>-17</v>
       </c>
       <c r="B65">
-        <v>-1.04</v>
+        <v>-0.92</v>
       </c>
       <c r="K65">
         <v>-26</v>
@@ -5290,7 +5290,7 @@
         <v>-16</v>
       </c>
       <c r="B66">
-        <v>-1.1499999999999999</v>
+        <v>-1.02</v>
       </c>
       <c r="K66">
         <v>-24</v>
@@ -5304,7 +5304,7 @@
         <v>-15</v>
       </c>
       <c r="B67">
-        <v>-1.2</v>
+        <v>-1.04</v>
       </c>
       <c r="K67">
         <v>-22</v>
@@ -5318,7 +5318,7 @@
         <v>-14</v>
       </c>
       <c r="B68">
-        <v>-1.18</v>
+        <v>-1.02</v>
       </c>
       <c r="K68">
         <v>-20</v>
@@ -5332,7 +5332,7 @@
         <v>-13</v>
       </c>
       <c r="B69">
-        <v>-1.1499999999999999</v>
+        <v>-0.98</v>
       </c>
       <c r="K69">
         <v>-18</v>
@@ -5346,7 +5346,7 @@
         <v>-12</v>
       </c>
       <c r="B70">
-        <v>-1.1100000000000001</v>
+        <v>-0.94</v>
       </c>
       <c r="K70">
         <v>-16</v>
@@ -5360,7 +5360,7 @@
         <v>-10</v>
       </c>
       <c r="B71">
-        <v>-0.99</v>
+        <v>-0.82</v>
       </c>
       <c r="K71">
         <v>-14</v>
@@ -5374,7 +5374,7 @@
         <v>-8</v>
       </c>
       <c r="B72">
-        <v>-0.84</v>
+        <v>-0.68</v>
       </c>
       <c r="K72">
         <v>-12</v>
@@ -5388,7 +5388,7 @@
         <v>-6</v>
       </c>
       <c r="B73">
-        <v>-0.69</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="K73">
         <v>-10</v>
@@ -5402,7 +5402,7 @@
         <v>-4</v>
       </c>
       <c r="B74">
-        <v>-0.48</v>
+        <v>-0.4</v>
       </c>
       <c r="K74">
         <v>-8</v>
@@ -5416,7 +5416,7 @@
         <v>-2</v>
       </c>
       <c r="B75">
-        <v>-0.25</v>
+        <v>-0.2</v>
       </c>
       <c r="K75">
         <v>-6</v>
@@ -5444,7 +5444,7 @@
         <v>2</v>
       </c>
       <c r="B77">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="K77">
         <v>-2</v>
@@ -5458,7 +5458,7 @@
         <v>4</v>
       </c>
       <c r="B78">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -5472,7 +5472,7 @@
         <v>6</v>
       </c>
       <c r="B79">
-        <v>0.69</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K79">
         <v>2</v>
@@ -5486,7 +5486,7 @@
         <v>8</v>
       </c>
       <c r="B80">
-        <v>0.84</v>
+        <v>0.68</v>
       </c>
       <c r="K80">
         <v>4</v>
@@ -5500,7 +5500,7 @@
         <v>10</v>
       </c>
       <c r="B81">
-        <v>0.99</v>
+        <v>0.82</v>
       </c>
       <c r="K81">
         <v>6</v>
@@ -5514,7 +5514,7 @@
         <v>12</v>
       </c>
       <c r="B82">
-        <v>1.1100000000000001</v>
+        <v>0.94</v>
       </c>
       <c r="K82">
         <v>8</v>
@@ -5528,7 +5528,7 @@
         <v>13</v>
       </c>
       <c r="B83">
-        <v>1.1499999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="K83">
         <v>10</v>
@@ -5542,7 +5542,7 @@
         <v>14</v>
       </c>
       <c r="B84">
-        <v>1.18</v>
+        <v>1.02</v>
       </c>
       <c r="K84">
         <v>12</v>
@@ -5556,7 +5556,7 @@
         <v>15</v>
       </c>
       <c r="B85">
-        <v>1.2</v>
+        <v>1.04</v>
       </c>
       <c r="K85">
         <v>14</v>
@@ -5570,7 +5570,7 @@
         <v>16</v>
       </c>
       <c r="B86">
-        <v>1.1499999999999999</v>
+        <v>1.02</v>
       </c>
       <c r="K86">
         <v>16</v>
@@ -5584,7 +5584,7 @@
         <v>17</v>
       </c>
       <c r="B87">
-        <v>1.04</v>
+        <v>0.92</v>
       </c>
       <c r="K87">
         <v>18</v>
@@ -5598,7 +5598,7 @@
         <v>18</v>
       </c>
       <c r="B88">
-        <v>0.78</v>
+        <v>0.71</v>
       </c>
       <c r="K88">
         <v>20</v>

</xml_diff>

<commit_message>
added extra creative mode wands
instant repair, refill all, refill weapons, refill fuel
</commit_message>
<xml_diff>
--- a/aoa_graphs/aoa_graphs.xlsx
+++ b/aoa_graphs/aoa_graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1whoh\Files\Creative\Minecrap\Mod_Develope\DiamondStarCombat\aoa_graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58775F2F-0EE5-4286-90F2-F98950644DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CB7E2E-F6CD-4237-A768-F43E182C0E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5655" yWindow="1425" windowWidth="17190" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4695" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4706,7 +4706,7 @@
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>